<commit_message>
UPDATED OUTPUT FILES AFTER CORRECTION OF ZP D AND ZP S INVERSION
(ZP D and ZP S were inverted in the input file, after the correction I had to rerun all the analyses to get the correct output files)
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/plits_ext_df.xlsx
+++ b/Multi-taxa_data/PLITs/plits_ext_df.xlsx
@@ -33680,10 +33680,10 @@
         </is>
       </c>
       <c r="B758">
-        <v>0</v>
+        <v>2165</v>
       </c>
       <c r="C758">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D758" t="inlineStr">
         <is>
@@ -33714,7 +33714,7 @@
         <v>1</v>
       </c>
       <c r="J758">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="759">
@@ -33768,10 +33768,10 @@
         </is>
       </c>
       <c r="B760">
-        <v>956</v>
+        <v>455</v>
       </c>
       <c r="C760">
-        <v>0.86</v>
+        <v>0.168</v>
       </c>
       <c r="D760" t="inlineStr">
         <is>
@@ -33802,7 +33802,7 @@
         <v>1</v>
       </c>
       <c r="J760">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="761">
@@ -33988,10 +33988,10 @@
         </is>
       </c>
       <c r="B765">
-        <v>120</v>
+        <v>9</v>
       </c>
       <c r="C765">
-        <v>0.108</v>
+        <v>0.003</v>
       </c>
       <c r="D765" t="inlineStr">
         <is>
@@ -34022,7 +34022,7 @@
         <v>1</v>
       </c>
       <c r="J765">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="766">
@@ -34032,10 +34032,10 @@
         </is>
       </c>
       <c r="B766">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C766">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="D766" t="inlineStr">
         <is>
@@ -34120,10 +34120,10 @@
         </is>
       </c>
       <c r="B768">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C768">
-        <v>0.024</v>
+        <v>0.012</v>
       </c>
       <c r="D768" t="inlineStr">
         <is>
@@ -34154,7 +34154,7 @@
         <v>1</v>
       </c>
       <c r="J768">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="769">
@@ -34164,10 +34164,10 @@
         </is>
       </c>
       <c r="B769">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C769">
-        <v>0.007</v>
+        <v>0.003</v>
       </c>
       <c r="D769" t="inlineStr">
         <is>
@@ -34208,10 +34208,10 @@
         </is>
       </c>
       <c r="B770">
-        <v>1222</v>
+        <v>2213</v>
       </c>
       <c r="C770">
-        <v>0.474</v>
+        <v>0.855</v>
       </c>
       <c r="D770" t="inlineStr">
         <is>
@@ -34242,7 +34242,7 @@
         <v>2</v>
       </c>
       <c r="J770">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="771">
@@ -34296,10 +34296,10 @@
         </is>
       </c>
       <c r="B772">
-        <v>1069</v>
+        <v>259</v>
       </c>
       <c r="C772">
-        <v>0.415</v>
+        <v>0.1</v>
       </c>
       <c r="D772" t="inlineStr">
         <is>
@@ -34330,7 +34330,7 @@
         <v>2</v>
       </c>
       <c r="J772">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="773">
@@ -34340,10 +34340,10 @@
         </is>
       </c>
       <c r="B773">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C773">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="D773" t="inlineStr">
         <is>
@@ -34516,10 +34516,10 @@
         </is>
       </c>
       <c r="B777">
-        <v>128</v>
+        <v>81</v>
       </c>
       <c r="C777">
-        <v>0.05</v>
+        <v>0.031</v>
       </c>
       <c r="D777" t="inlineStr">
         <is>
@@ -34550,7 +34550,7 @@
         <v>2</v>
       </c>
       <c r="J777">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="778">
@@ -34560,10 +34560,10 @@
         </is>
       </c>
       <c r="B778">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C778">
-        <v>0.013</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="D778" t="inlineStr">
         <is>
@@ -34648,10 +34648,10 @@
         </is>
       </c>
       <c r="B780">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C780">
-        <v>0.044</v>
+        <v>0.003</v>
       </c>
       <c r="D780" t="inlineStr">
         <is>
@@ -34682,7 +34682,7 @@
         <v>2</v>
       </c>
       <c r="J780">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="781">
@@ -34692,10 +34692,10 @@
         </is>
       </c>
       <c r="B781">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C781">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="D781" t="inlineStr">
         <is>
@@ -34736,10 +34736,10 @@
         </is>
       </c>
       <c r="B782">
-        <v>1479</v>
+        <v>2440</v>
       </c>
       <c r="C782">
-        <v>0.546</v>
+        <v>0.901</v>
       </c>
       <c r="D782" t="inlineStr">
         <is>
@@ -34770,7 +34770,7 @@
         <v>3</v>
       </c>
       <c r="J782">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="783">
@@ -34824,10 +34824,10 @@
         </is>
       </c>
       <c r="B784">
-        <v>1136</v>
+        <v>127</v>
       </c>
       <c r="C784">
-        <v>0.419</v>
+        <v>0.047</v>
       </c>
       <c r="D784" t="inlineStr">
         <is>
@@ -34858,7 +34858,7 @@
         <v>3</v>
       </c>
       <c r="J784">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="785">
@@ -34912,10 +34912,10 @@
         </is>
       </c>
       <c r="B786">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C786">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="D786" t="inlineStr">
         <is>
@@ -35044,10 +35044,10 @@
         </is>
       </c>
       <c r="B789">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C789">
-        <v>0.005</v>
+        <v>0.021</v>
       </c>
       <c r="D789" t="inlineStr">
         <is>
@@ -35078,7 +35078,7 @@
         <v>3</v>
       </c>
       <c r="J789">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="790">
@@ -35088,10 +35088,10 @@
         </is>
       </c>
       <c r="B790">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C790">
-        <v>0.021</v>
+        <v>0.024</v>
       </c>
       <c r="D790" t="inlineStr">
         <is>
@@ -35132,10 +35132,10 @@
         </is>
       </c>
       <c r="B791">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C791">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D791" t="inlineStr">
         <is>
@@ -35176,10 +35176,10 @@
         </is>
       </c>
       <c r="B792">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C792">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="D792" t="inlineStr">
         <is>
@@ -35210,7 +35210,7 @@
         <v>3</v>
       </c>
       <c r="J792">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="793">
@@ -35220,10 +35220,10 @@
         </is>
       </c>
       <c r="B793">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C793">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="D793" t="inlineStr">
         <is>
@@ -35264,10 +35264,10 @@
         </is>
       </c>
       <c r="B794">
-        <v>2165</v>
+        <v>0</v>
       </c>
       <c r="C794">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D794" t="inlineStr">
         <is>
@@ -35298,7 +35298,7 @@
         <v>1</v>
       </c>
       <c r="J794">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="795">
@@ -35352,10 +35352,10 @@
         </is>
       </c>
       <c r="B796">
-        <v>455</v>
+        <v>956</v>
       </c>
       <c r="C796">
-        <v>0.168</v>
+        <v>0.86</v>
       </c>
       <c r="D796" t="inlineStr">
         <is>
@@ -35386,7 +35386,7 @@
         <v>1</v>
       </c>
       <c r="J796">
-        <v>0.06</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="797">
@@ -35572,10 +35572,10 @@
         </is>
       </c>
       <c r="B801">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="C801">
-        <v>0.003</v>
+        <v>0.108</v>
       </c>
       <c r="D801" t="inlineStr">
         <is>
@@ -35606,7 +35606,7 @@
         <v>1</v>
       </c>
       <c r="J801">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="802">
@@ -35616,10 +35616,10 @@
         </is>
       </c>
       <c r="B802">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C802">
-        <v>0.013</v>
+        <v>0</v>
       </c>
       <c r="D802" t="inlineStr">
         <is>
@@ -35704,10 +35704,10 @@
         </is>
       </c>
       <c r="B804">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C804">
-        <v>0.012</v>
+        <v>0.024</v>
       </c>
       <c r="D804" t="inlineStr">
         <is>
@@ -35738,7 +35738,7 @@
         <v>1</v>
       </c>
       <c r="J804">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="805">
@@ -35748,10 +35748,10 @@
         </is>
       </c>
       <c r="B805">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C805">
-        <v>0.003</v>
+        <v>0.007</v>
       </c>
       <c r="D805" t="inlineStr">
         <is>
@@ -35792,10 +35792,10 @@
         </is>
       </c>
       <c r="B806">
-        <v>2213</v>
+        <v>1222</v>
       </c>
       <c r="C806">
-        <v>0.855</v>
+        <v>0.474</v>
       </c>
       <c r="D806" t="inlineStr">
         <is>
@@ -35826,7 +35826,7 @@
         <v>2</v>
       </c>
       <c r="J806">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="807">
@@ -35880,10 +35880,10 @@
         </is>
       </c>
       <c r="B808">
-        <v>259</v>
+        <v>1069</v>
       </c>
       <c r="C808">
-        <v>0.1</v>
+        <v>0.415</v>
       </c>
       <c r="D808" t="inlineStr">
         <is>
@@ -35914,7 +35914,7 @@
         <v>2</v>
       </c>
       <c r="J808">
-        <v>0.06</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="809">
@@ -35924,10 +35924,10 @@
         </is>
       </c>
       <c r="B809">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C809">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="D809" t="inlineStr">
         <is>
@@ -36100,10 +36100,10 @@
         </is>
       </c>
       <c r="B813">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C813">
-        <v>0.031</v>
+        <v>0.05</v>
       </c>
       <c r="D813" t="inlineStr">
         <is>
@@ -36134,7 +36134,7 @@
         <v>2</v>
       </c>
       <c r="J813">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="814">
@@ -36144,10 +36144,10 @@
         </is>
       </c>
       <c r="B814">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C814">
-        <v>0.008999999999999999</v>
+        <v>0.013</v>
       </c>
       <c r="D814" t="inlineStr">
         <is>
@@ -36232,10 +36232,10 @@
         </is>
       </c>
       <c r="B816">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C816">
-        <v>0.003</v>
+        <v>0.044</v>
       </c>
       <c r="D816" t="inlineStr">
         <is>
@@ -36266,7 +36266,7 @@
         <v>2</v>
       </c>
       <c r="J816">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="817">
@@ -36276,10 +36276,10 @@
         </is>
       </c>
       <c r="B817">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C817">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="D817" t="inlineStr">
         <is>
@@ -36320,10 +36320,10 @@
         </is>
       </c>
       <c r="B818">
-        <v>2440</v>
+        <v>1479</v>
       </c>
       <c r="C818">
-        <v>0.901</v>
+        <v>0.546</v>
       </c>
       <c r="D818" t="inlineStr">
         <is>
@@ -36354,7 +36354,7 @@
         <v>3</v>
       </c>
       <c r="J818">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="819">
@@ -36408,10 +36408,10 @@
         </is>
       </c>
       <c r="B820">
-        <v>127</v>
+        <v>1136</v>
       </c>
       <c r="C820">
-        <v>0.047</v>
+        <v>0.419</v>
       </c>
       <c r="D820" t="inlineStr">
         <is>
@@ -36442,7 +36442,7 @@
         <v>3</v>
       </c>
       <c r="J820">
-        <v>0.06</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="821">
@@ -36496,10 +36496,10 @@
         </is>
       </c>
       <c r="B822">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C822">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="D822" t="inlineStr">
         <is>
@@ -36628,10 +36628,10 @@
         </is>
       </c>
       <c r="B825">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C825">
-        <v>0.021</v>
+        <v>0.005</v>
       </c>
       <c r="D825" t="inlineStr">
         <is>
@@ -36662,7 +36662,7 @@
         <v>3</v>
       </c>
       <c r="J825">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="826">
@@ -36672,10 +36672,10 @@
         </is>
       </c>
       <c r="B826">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C826">
-        <v>0.024</v>
+        <v>0.021</v>
       </c>
       <c r="D826" t="inlineStr">
         <is>
@@ -36716,10 +36716,10 @@
         </is>
       </c>
       <c r="B827">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C827">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="D827" t="inlineStr">
         <is>
@@ -36760,10 +36760,10 @@
         </is>
       </c>
       <c r="B828">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C828">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="D828" t="inlineStr">
         <is>
@@ -36794,7 +36794,7 @@
         <v>3</v>
       </c>
       <c r="J828">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="829">
@@ -36804,10 +36804,10 @@
         </is>
       </c>
       <c r="B829">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C829">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="D829" t="inlineStr">
         <is>

</xml_diff>